<commit_message>
updates for test scripts
</commit_message>
<xml_diff>
--- a/Test/ExploratoryTesting_(Checklist).xlsx
+++ b/Test/ExploratoryTesting_(Checklist).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\engineering\ceg team2\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481FAD1C-5D06-46F0-8328-1D143287AA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50C2FFE-94E8-4FA2-8AA8-09B78DE0EA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,13 +90,13 @@
     <t>Verify the page is responsive and displays correctly on different devices.</t>
   </si>
   <si>
-    <t>Verify the search field handles special characters.</t>
-  </si>
-  <si>
     <t>Verify the application displays an appropriate message when no search results are found.</t>
   </si>
   <si>
     <t>Ready</t>
+  </si>
+  <si>
+    <t>Verify the search field handles different languages</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -527,7 +527,7 @@
   <dimension ref="B2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -580,12 +580,12 @@
         <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <f t="shared" ref="B5:B19" si="0">B4+1</f>
+        <f t="shared" ref="B5:B17" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -595,7 +595,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -637,10 +637,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -652,10 +652,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update manual test cases
</commit_message>
<xml_diff>
--- a/Test/ExploratoryTesting_(Checklist).xlsx
+++ b/Test/ExploratoryTesting_(Checklist).xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\engineering\ceg team2\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cegedim Intership\Desktop\movie-db\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50C2FFE-94E8-4FA2-8AA8-09B78DE0EA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t>Tc_N</t>
   </si>
@@ -60,9 +59,6 @@
     <t>Movie List Display</t>
   </si>
   <si>
-    <t>Verify the list of movies is displayed on the page.</t>
-  </si>
-  <si>
     <t>Verify each movie in the list has a title and thumbnail.</t>
   </si>
   <si>
@@ -97,12 +93,58 @@
   </si>
   <si>
     <t>Verify the search field handles different languages</t>
+  </si>
+  <si>
+    <t>Verify searching with "Enter" button</t>
+  </si>
+  <si>
+    <t>Verify searching with clicking on the search icon with mouse</t>
+  </si>
+  <si>
+    <t>Verify the application checks the local database when a movie is clicked.</t>
+  </si>
+  <si>
+    <t>Verify the application retrieves and displays movie details from the local database if available.</t>
+  </si>
+  <si>
+    <t>Verify the application calls the API to fetch movie details if not found in the local database.</t>
+  </si>
+  <si>
+    <t>Verify the application does not call the API to fetch movie details if  found in the local database.</t>
+  </si>
+  <si>
+    <t>Verify the application saves the fetched movie details from API to the local database.</t>
+  </si>
+  <si>
+    <t>Movie DB Verification</t>
+  </si>
+  <si>
+    <t>Verify the list of movies is displayed on the page (20 movies) .</t>
+  </si>
+  <si>
+    <t>Verify the application uses the API to load the 20 popular movies when the page is first loaded.</t>
+  </si>
+  <si>
+    <t>Verify the application uses the API to search for movies based on the search input.</t>
+  </si>
+  <si>
+    <t>Verify the movie details are saved correctly in local DB after fetch it from the API</t>
+  </si>
+  <si>
+    <t>Verify the application save data of the movie details in local DB if its fetched from the API only
+(Like it does not dublicate it in DB if it was already fetched from local DB)</t>
+  </si>
+  <si>
+    <t>Verify the application displays an appropriate error message if the API call fails</t>
+  </si>
+  <si>
+    <t>Fetching from API</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,7 +173,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +201,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,17 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -243,6 +295,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,280 +605,458 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="84" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:5" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
+    <row r="3" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+      <c r="E3" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <f t="shared" ref="B5:B30" si="0">B4+1</f>
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <f t="shared" ref="B5:B17" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="E8" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E19" xr:uid="{2CBAC202-845C-4A0C-861B-895714E3BA1C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E30">
       <formula1>"Pass,Fail,Ready"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update manual test cases ( add load button )
</commit_message>
<xml_diff>
--- a/Test/ExploratoryTesting_(Checklist).xlsx
+++ b/Test/ExploratoryTesting_(Checklist).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t>Tc_N</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>Fetching from API</t>
+  </si>
+  <si>
+    <t>Load button</t>
+  </si>
+  <si>
+    <t>Verify load button appear in the ui</t>
+  </si>
+  <si>
+    <t>verify when click on load button the number of movies in the list increase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify click in the load button 3 times </t>
   </si>
 </sst>
 </file>
@@ -606,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E30"/>
+  <dimension ref="B2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="76" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +679,7 @@
     </row>
     <row r="5" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <f t="shared" ref="B5:B30" si="0">B4+1</f>
+        <f t="shared" ref="B5:B34" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1045,14 +1057,62 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="12"/>
+      <c r="C30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E34">
       <formula1>"Pass,Fail,Ready"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add search for vaild movie as a bdd scenario in the automation script
</commit_message>
<xml_diff>
--- a/Test/ExploratoryTesting_(Checklist).xlsx
+++ b/Test/ExploratoryTesting_(Checklist).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
   <si>
     <t>Tc_N</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t xml:space="preserve">Verify click in the load button 3 times </t>
+  </si>
+  <si>
+    <t>Verify searching for the product with different cases ( capital letters and small letters )</t>
   </si>
 </sst>
 </file>
@@ -618,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E34"/>
+  <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="76" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="76" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +682,7 @@
     </row>
     <row r="5" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <f t="shared" ref="B5:B34" si="0">B4+1</f>
+        <f t="shared" ref="B5:B33" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -787,11 +790,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>31</v>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>21</v>
@@ -806,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>21</v>
@@ -817,11 +820,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>13</v>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>21</v>
@@ -836,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>21</v>
@@ -851,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>21</v>
@@ -866,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>21</v>
@@ -877,11 +880,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>18</v>
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>21</v>
@@ -896,7 +899,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>21</v>
@@ -907,11 +910,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>25</v>
+      <c r="C20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>21</v>
@@ -926,13 +929,13 @@
         <v>30</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -941,7 +944,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>21</v>
@@ -956,7 +959,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>21</v>
@@ -971,7 +974,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>21</v>
@@ -986,7 +989,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>21</v>
@@ -997,11 +1000,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>32</v>
+      <c r="C26" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>21</v>
@@ -1016,13 +1019,13 @@
         <v>37</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1030,14 +1033,14 @@
       <c r="C28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>35</v>
+      <c r="D28" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1045,8 +1048,8 @@
       <c r="C29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>36</v>
+      <c r="D29" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>21</v>
@@ -1057,11 +1060,11 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>39</v>
+      <c r="C30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>21</v>
@@ -1076,7 +1079,7 @@
         <v>38</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>21</v>
@@ -1091,17 +1094,26 @@
         <v>38</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
@@ -1109,10 +1121,16 @@
       <c r="D34" s="3"/>
       <c r="E34" s="12"/>
     </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E35">
       <formula1>"Pass,Fail,Ready"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>